<commit_message>
Simplified Assertion-Reduce Code Complexity
</commit_message>
<xml_diff>
--- a/Excel/Registration.xlsx
+++ b/Excel/Registration.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fardi\PycharmProjects\OpenCart Automation Project\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4759C8-9A88-4486-8D19-09AEBBA6B609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEB55D7-F840-4372-A441-4AD87B050EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{811FDAB8-D69D-4AA4-925F-635022892DBA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Registration" sheetId="1" r:id="rId1"/>
-    <sheet name="Login" sheetId="3" r:id="rId2"/>
+    <sheet name="Registration-valid" sheetId="1" r:id="rId1"/>
+    <sheet name="Registration-invalid" sheetId="5" r:id="rId2"/>
+    <sheet name="Login-valid" sheetId="3" r:id="rId3"/>
+    <sheet name="Login-invalid" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>firstname</t>
   </si>
@@ -52,13 +54,25 @@
     <t>ratul##2211@xxgrd</t>
   </si>
   <si>
-    <t>dwddcacawfef</t>
-  </si>
-  <si>
-    <t>wwefwfewfw@fved.com</t>
-  </si>
-  <si>
     <t>miao@gmail.com</t>
+  </si>
+  <si>
+    <t>11111@gmail.com</t>
+  </si>
+  <si>
+    <t>dcvnskjdvnkjsnvdjkn</t>
+  </si>
+  <si>
+    <t>Fardin</t>
+  </si>
+  <si>
+    <t>Ahosan</t>
+  </si>
+  <si>
+    <t>fardinahosan@gmail.com</t>
+  </si>
+  <si>
+    <t>uyeguyegcuecvwcegv</t>
   </si>
 </sst>
 </file>
@@ -444,7 +458,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -464,33 +479,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{8291EF2D-9926-4062-88C5-8BC2C04462B7}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{5FFD4C2F-A99D-4752-8D62-4C2A670CC854}"/>
+    <hyperlink ref="D2" r:id="rId2" display="ratul##2211@xxgrd" xr:uid="{5FFD4C2F-A99D-4752-8D62-4C2A670CC854}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B88AB4-002B-425D-8BD9-8D9D4CA4C899}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FC504E-AAB0-4295-9CBF-911D160B99E8}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{27B13F4F-A65A-4681-BF9D-2A70A15E99F1}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{440535E3-D4BD-4D84-B3D1-7BDD06D03A98}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B88AB4-002B-425D-8BD9-8D9D4CA4C899}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,26 +577,53 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="miao@gmail.com" xr:uid="{2BD68A7F-E8C1-4243-86F2-8D82C759E136}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{505E9D41-8EDA-4AAD-BBFD-57517EBFF1A1}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{51432B83-006D-45A0-A139-ACCB15F14FF1}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{C3E8B480-5B95-45E4-AE60-9A0BE6699381}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{51432B83-006D-45A0-A139-ACCB15F14FF1}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C3E8B480-5B95-45E4-AE60-9A0BE6699381}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFDD5EB-719C-463D-B58B-3DAD5EB96D1B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{77853B23-CF13-4494-9B46-26BD5217F3E7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed : element not found
</commit_message>
<xml_diff>
--- a/Excel/Registration.xlsx
+++ b/Excel/Registration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fardi\PycharmProjects\OpenCart Automation Project\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2812BB52-7AE0-465E-9C31-859C1504C391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EEF976-93C1-4D09-B316-798B06D70D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{811FDAB8-D69D-4AA4-925F-635022892DBA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{811FDAB8-D69D-4AA4-925F-635022892DBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration-valid" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>firstname</t>
   </si>
@@ -70,12 +70,6 @@
     <t>Ahosan</t>
   </si>
   <si>
-    <t>fardinahosan@gmail.com</t>
-  </si>
-  <si>
-    <t>uyeguyegcuecvwcegv</t>
-  </si>
-  <si>
     <t>lastname</t>
   </si>
   <si>
@@ -92,6 +86,18 @@
   </si>
   <si>
     <t>Rajshahi</t>
+  </si>
+  <si>
+    <t>Fardinddppp</t>
+  </si>
+  <si>
+    <t>Akjnjkhosandd</t>
+  </si>
+  <si>
+    <t>fardinahhosan@gmail.comd</t>
+  </si>
+  <si>
+    <t>uyeguyegcuecvwcellgvdd</t>
   </si>
 </sst>
 </file>
@@ -478,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685D3AFF-46A3-494C-89CE-C074C7B86193}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -505,16 +511,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -659,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77531C4F-BA09-4ADE-8935-933D8CF66C85}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,16 +681,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -695,10 +701,10 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>6100</v>

</xml_diff>